<commit_message>
solve issue phone number
</commit_message>
<xml_diff>
--- a/pybangla/report/eval_data_2.11.7_v2.xlsx
+++ b/pybangla/report/eval_data_2.11.7_v2.xlsx
@@ -583,7 +583,7 @@
         <v>8</v>
       </c>
       <c r="N2" t="n">
-        <v>14.14</v>
+        <v>13.03</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="N3" t="n">
-        <v>0.71</v>
+        <v>0.85</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -703,7 +703,7 @@
         <v>9</v>
       </c>
       <c r="N4" t="n">
-        <v>0.38</v>
+        <v>0.48</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -763,7 +763,7 @@
         <v>9</v>
       </c>
       <c r="N5" t="n">
-        <v>0.42</v>
+        <v>0.51</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -823,7 +823,7 @@
         <v>12</v>
       </c>
       <c r="N6" t="n">
-        <v>2.53</v>
+        <v>1.04</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -883,7 +883,7 @@
         <v>11</v>
       </c>
       <c r="N7" t="n">
-        <v>0.75</v>
+        <v>0.68</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>13</v>
       </c>
       <c r="N8" t="n">
-        <v>0.7</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="N9" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.46</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
       <c r="N10" t="n">
-        <v>0.57</v>
+        <v>0.45</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1115,7 +1115,7 @@
         <v>9</v>
       </c>
       <c r="N11" t="n">
-        <v>0.43</v>
+        <v>0.35</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1175,7 +1175,7 @@
         <v>12</v>
       </c>
       <c r="N12" t="n">
-        <v>0.87</v>
+        <v>0.61</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1235,7 +1235,7 @@
         <v>10</v>
       </c>
       <c r="N13" t="n">
-        <v>0.5</v>
+        <v>0.41</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1291,7 +1291,7 @@
         <v>10</v>
       </c>
       <c r="N14" t="n">
-        <v>0.35</v>
+        <v>0.32</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
         <v>12</v>
       </c>
       <c r="N15" t="n">
-        <v>0.55</v>
+        <v>0.52</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1411,7 +1411,7 @@
         <v>11</v>
       </c>
       <c r="N16" t="n">
-        <v>0.42</v>
+        <v>0.35</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1471,7 +1471,7 @@
         <v>10</v>
       </c>
       <c r="N17" t="n">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1527,7 +1527,7 @@
         <v>10</v>
       </c>
       <c r="N18" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1587,7 +1587,7 @@
         <v>11</v>
       </c>
       <c r="N19" t="n">
-        <v>0.63</v>
+        <v>0.66</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="N20" t="n">
-        <v>0.36</v>
+        <v>0.39</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1767,7 +1767,7 @@
         <v>11</v>
       </c>
       <c r="N22" t="n">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2067,7 +2067,7 @@
         <v>11</v>
       </c>
       <c r="N27" t="n">
-        <v>0.35</v>
+        <v>0.37</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2127,7 +2127,7 @@
         <v>10</v>
       </c>
       <c r="N28" t="n">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2247,7 +2247,7 @@
         <v>6</v>
       </c>
       <c r="N30" t="n">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
         <v>5</v>
       </c>
       <c r="N31" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2415,7 +2415,7 @@
         <v>9</v>
       </c>
       <c r="N33" t="n">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2475,7 +2475,7 @@
         <v>14</v>
       </c>
       <c r="N34" t="n">
-        <v>0.63</v>
+        <v>0.52</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2531,7 +2531,7 @@
         <v>29</v>
       </c>
       <c r="N35" t="n">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
         <v>35</v>
       </c>
       <c r="N36" t="n">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2643,7 +2643,7 @@
         <v>25</v>
       </c>
       <c r="N37" t="n">
-        <v>0.65</v>
+        <v>0.72</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -2699,7 +2699,7 @@
         <v>25</v>
       </c>
       <c r="N38" t="n">
-        <v>0.53</v>
+        <v>0.55</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2759,7 +2759,7 @@
         <v>12</v>
       </c>
       <c r="N39" t="n">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -2875,7 +2875,7 @@
         <v>14</v>
       </c>
       <c r="N41" t="n">
-        <v>0.54</v>
+        <v>0.51</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
         <v>5</v>
       </c>
       <c r="N43" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3043,7 +3043,7 @@
         <v>19</v>
       </c>
       <c r="N44" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3099,7 +3099,7 @@
         <v>14</v>
       </c>
       <c r="N45" t="n">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3155,7 +3155,7 @@
         <v>32</v>
       </c>
       <c r="N46" t="n">
-        <v>0.85</v>
+        <v>0.88</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3211,7 +3211,7 @@
         <v>19</v>
       </c>
       <c r="N47" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3323,7 +3323,7 @@
         <v>16</v>
       </c>
       <c r="N49" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -3379,7 +3379,7 @@
         <v>16</v>
       </c>
       <c r="N50" t="n">
-        <v>0.77</v>
+        <v>0.55</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -3439,7 +3439,7 @@
         <v>18</v>
       </c>
       <c r="N51" t="n">
-        <v>0.57</v>
+        <v>0.58</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -3495,7 +3495,7 @@
         <v>10</v>
       </c>
       <c r="N52" t="n">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -3551,7 +3551,7 @@
         <v>31</v>
       </c>
       <c r="N53" t="n">
-        <v>0.87</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -3607,7 +3607,7 @@
         <v>5</v>
       </c>
       <c r="N54" t="n">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -3663,7 +3663,7 @@
         <v>5</v>
       </c>
       <c r="N55" t="n">
-        <v>0.24</v>
+        <v>0.28</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -3719,7 +3719,7 @@
         <v>19</v>
       </c>
       <c r="N56" t="n">
-        <v>0.7</v>
+        <v>0.64</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -3775,7 +3775,7 @@
         <v>14</v>
       </c>
       <c r="N57" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -3831,7 +3831,7 @@
         <v>110</v>
       </c>
       <c r="N58" t="n">
-        <v>2.2</v>
+        <v>2.23</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
         <v>10</v>
       </c>
       <c r="N59" t="n">
-        <v>0.75</v>
+        <v>0.66</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -3947,7 +3947,7 @@
         <v>17</v>
       </c>
       <c r="N60" t="n">
-        <v>1.27</v>
+        <v>1.24</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4007,7 +4007,7 @@
         <v>46</v>
       </c>
       <c r="N61" t="n">
-        <v>1.03</v>
+        <v>1.01</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
         <v>43</v>
       </c>
       <c r="N62" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -4119,7 +4119,7 @@
         <v>33</v>
       </c>
       <c r="N63" t="n">
-        <v>1.23</v>
+        <v>0.86</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -4175,7 +4175,7 @@
         <v>31</v>
       </c>
       <c r="N64" t="n">
-        <v>0.88</v>
+        <v>0.73</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -4231,7 +4231,7 @@
         <v>36</v>
       </c>
       <c r="N65" t="n">
-        <v>1.07</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -4287,7 +4287,7 @@
         <v>59</v>
       </c>
       <c r="N66" t="n">
-        <v>1.2</v>
+        <v>1.23</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -4343,7 +4343,7 @@
         <v>19</v>
       </c>
       <c r="N67" t="n">
-        <v>0.68</v>
+        <v>0.59</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -4399,7 +4399,7 @@
         <v>30</v>
       </c>
       <c r="N68" t="n">
-        <v>1</v>
+        <v>0.71</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -4455,7 +4455,7 @@
         <v>32</v>
       </c>
       <c r="N69" t="n">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -4511,7 +4511,7 @@
         <v>6</v>
       </c>
       <c r="N70" t="n">
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -4567,7 +4567,7 @@
         <v>5</v>
       </c>
       <c r="N71" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -4627,7 +4627,7 @@
         <v>2</v>
       </c>
       <c r="N72" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -4687,7 +4687,7 @@
         <v>2</v>
       </c>
       <c r="N73" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -4747,7 +4747,7 @@
         <v>4</v>
       </c>
       <c r="N74" t="n">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
         <v>13</v>
       </c>
       <c r="N75" t="n">
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -4859,7 +4859,7 @@
         <v>13</v>
       </c>
       <c r="N76" t="n">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -4915,7 +4915,7 @@
         <v>14</v>
       </c>
       <c r="N77" t="n">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -4971,7 +4971,7 @@
         <v>13</v>
       </c>
       <c r="N78" t="n">
-        <v>0.48</v>
+        <v>0.43</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -5027,7 +5027,7 @@
         <v>13</v>
       </c>
       <c r="N79" t="n">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -5083,7 +5083,7 @@
         <v>14</v>
       </c>
       <c r="N80" t="n">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -5139,7 +5139,7 @@
         <v>13</v>
       </c>
       <c r="N81" t="n">
-        <v>0.46</v>
+        <v>0.43</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -5195,7 +5195,7 @@
         <v>13</v>
       </c>
       <c r="N82" t="n">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -5251,7 +5251,7 @@
         <v>13</v>
       </c>
       <c r="N83" t="n">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -5307,7 +5307,7 @@
         <v>13</v>
       </c>
       <c r="N84" t="n">
-        <v>0.7</v>
+        <v>0.42</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -5363,7 +5363,7 @@
         <v>13</v>
       </c>
       <c r="N85" t="n">
-        <v>0.75</v>
+        <v>0.41</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -5419,7 +5419,7 @@
         <v>14</v>
       </c>
       <c r="N86" t="n">
-        <v>0.51</v>
+        <v>0.4</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -5475,7 +5475,7 @@
         <v>13</v>
       </c>
       <c r="N87" t="n">
-        <v>0.53</v>
+        <v>0.42</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -5531,7 +5531,7 @@
         <v>13</v>
       </c>
       <c r="N88" t="n">
-        <v>0.55</v>
+        <v>0.43</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -5587,7 +5587,7 @@
         <v>13</v>
       </c>
       <c r="N89" t="n">
-        <v>0.47</v>
+        <v>0.37</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
@@ -5643,7 +5643,7 @@
         <v>14</v>
       </c>
       <c r="N90" t="n">
-        <v>0.5</v>
+        <v>0.42</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -5699,7 +5699,7 @@
         <v>14</v>
       </c>
       <c r="N91" t="n">
-        <v>0.61</v>
+        <v>0.41</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -5755,7 +5755,7 @@
         <v>14</v>
       </c>
       <c r="N92" t="n">
-        <v>0.45</v>
+        <v>0.41</v>
       </c>
       <c r="O92" t="inlineStr">
         <is>
@@ -5811,7 +5811,7 @@
         <v>14</v>
       </c>
       <c r="N93" t="n">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
@@ -5867,7 +5867,7 @@
         <v>35</v>
       </c>
       <c r="N94" t="n">
-        <v>0.74</v>
+        <v>0.72</v>
       </c>
       <c r="O94" t="inlineStr">
         <is>
@@ -5927,7 +5927,7 @@
         <v>4</v>
       </c>
       <c r="N95" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6039,7 +6039,7 @@
         <v>149</v>
       </c>
       <c r="N97" t="n">
-        <v>2.65</v>
+        <v>2.53</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6099,7 +6099,7 @@
         <v>15</v>
       </c>
       <c r="N98" t="n">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6155,7 +6155,7 @@
         <v>15</v>
       </c>
       <c r="N99" t="n">
-        <v>0.57</v>
+        <v>0.36</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6211,7 +6211,7 @@
         <v>12</v>
       </c>
       <c r="N100" t="n">
-        <v>0.31</v>
+        <v>0.29</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6267,7 +6267,7 @@
         <v>5</v>
       </c>
       <c r="N101" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -6379,7 +6379,7 @@
         <v>5</v>
       </c>
       <c r="N103" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -6603,7 +6603,7 @@
         <v>5</v>
       </c>
       <c r="N107" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -6659,7 +6659,7 @@
         <v>6</v>
       </c>
       <c r="N108" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="O108" t="inlineStr">
         <is>
@@ -6771,7 +6771,7 @@
         <v>5</v>
       </c>
       <c r="N110" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7107,7 +7107,7 @@
         <v>8</v>
       </c>
       <c r="N116" t="n">
-        <v>0.28</v>
+        <v>0.27</v>
       </c>
       <c r="O116" t="inlineStr"/>
       <c r="P116" t="inlineStr"/>
@@ -7271,7 +7271,7 @@
         <v>6</v>
       </c>
       <c r="N119" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="O119" t="inlineStr">
         <is>
@@ -7383,7 +7383,7 @@
         <v>6</v>
       </c>
       <c r="N121" t="n">
-        <v>0.42</v>
+        <v>0.26</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -7439,7 +7439,7 @@
         <v>9</v>
       </c>
       <c r="N122" t="n">
-        <v>0.49</v>
+        <v>0.31</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -7495,7 +7495,7 @@
         <v>5</v>
       </c>
       <c r="N123" t="n">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -7551,7 +7551,7 @@
         <v>5</v>
       </c>
       <c r="N124" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -7663,7 +7663,7 @@
         <v>6</v>
       </c>
       <c r="N126" t="n">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -7719,7 +7719,7 @@
         <v>6</v>
       </c>
       <c r="N127" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -7775,7 +7775,7 @@
         <v>6</v>
       </c>
       <c r="N128" t="n">
-        <v>0.29</v>
+        <v>0.25</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -7887,7 +7887,7 @@
         <v>7</v>
       </c>
       <c r="N130" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -7943,7 +7943,7 @@
         <v>7</v>
       </c>
       <c r="N131" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -8111,7 +8111,7 @@
         <v>5</v>
       </c>
       <c r="N134" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -8223,7 +8223,7 @@
         <v>6</v>
       </c>
       <c r="N136" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="O136" t="inlineStr"/>
       <c r="P136" t="inlineStr"/>
@@ -8387,7 +8387,7 @@
         <v>5</v>
       </c>
       <c r="N139" t="n">
-        <v>0.4</v>
+        <v>0.32</v>
       </c>
       <c r="O139" t="inlineStr"/>
       <c r="P139" t="inlineStr">
@@ -8443,7 +8443,7 @@
         <v>6</v>
       </c>
       <c r="N140" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="O140" t="inlineStr"/>
       <c r="P140" t="inlineStr">
@@ -8551,7 +8551,7 @@
         <v>5</v>
       </c>
       <c r="N142" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -8663,7 +8663,7 @@
         <v>10</v>
       </c>
       <c r="N144" t="n">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -8719,7 +8719,7 @@
         <v>9</v>
       </c>
       <c r="N145" t="n">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -8879,7 +8879,7 @@
         <v>1</v>
       </c>
       <c r="N148" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="O148" t="inlineStr"/>
       <c r="P148" t="inlineStr"/>
@@ -8983,7 +8983,7 @@
         <v>10</v>
       </c>
       <c r="N150" t="n">
-        <v>0.35</v>
+        <v>0.32</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -9095,7 +9095,7 @@
         <v>6</v>
       </c>
       <c r="N152" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -9151,7 +9151,7 @@
         <v>29</v>
       </c>
       <c r="N153" t="n">
-        <v>0.72</v>
+        <v>0.73</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -9207,7 +9207,7 @@
         <v>55</v>
       </c>
       <c r="N154" t="n">
-        <v>1.28</v>
+        <v>1.04</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -9263,7 +9263,7 @@
         <v>10</v>
       </c>
       <c r="N155" t="n">
-        <v>0.45</v>
+        <v>0.41</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -9319,7 +9319,7 @@
         <v>9</v>
       </c>
       <c r="N156" t="n">
-        <v>0.54</v>
+        <v>0.4</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -9375,7 +9375,7 @@
         <v>10</v>
       </c>
       <c r="N157" t="n">
-        <v>0.54</v>
+        <v>0.36</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -9431,7 +9431,7 @@
         <v>12</v>
       </c>
       <c r="N158" t="n">
-        <v>0.66</v>
+        <v>0.43</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -9487,7 +9487,7 @@
         <v>11</v>
       </c>
       <c r="N159" t="n">
-        <v>0.54</v>
+        <v>0.41</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -9543,7 +9543,7 @@
         <v>10</v>
       </c>
       <c r="N160" t="n">
-        <v>0.68</v>
+        <v>0.39</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -9599,7 +9599,7 @@
         <v>11</v>
       </c>
       <c r="N161" t="n">
-        <v>0.72</v>
+        <v>0.39</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -9655,7 +9655,7 @@
         <v>10</v>
       </c>
       <c r="N162" t="n">
-        <v>0.67</v>
+        <v>0.4</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -9711,7 +9711,7 @@
         <v>10</v>
       </c>
       <c r="N163" t="n">
-        <v>0.63</v>
+        <v>0.42</v>
       </c>
       <c r="O163" t="inlineStr">
         <is>
@@ -9767,7 +9767,7 @@
         <v>9</v>
       </c>
       <c r="N164" t="n">
-        <v>0.55</v>
+        <v>0.36</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -9823,7 +9823,7 @@
         <v>10</v>
       </c>
       <c r="N165" t="n">
-        <v>0.65</v>
+        <v>0.38</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -9879,7 +9879,7 @@
         <v>10</v>
       </c>
       <c r="N166" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.42</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -9935,7 +9935,7 @@
         <v>10</v>
       </c>
       <c r="N167" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -9991,7 +9991,7 @@
         <v>10</v>
       </c>
       <c r="N168" t="n">
-        <v>0.51</v>
+        <v>0.41</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -10047,7 +10047,7 @@
         <v>15</v>
       </c>
       <c r="N169" t="n">
-        <v>0.45</v>
+        <v>0.38</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -10103,7 +10103,7 @@
         <v>11</v>
       </c>
       <c r="N170" t="n">
-        <v>0.4</v>
+        <v>0.34</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -10159,7 +10159,7 @@
         <v>5</v>
       </c>
       <c r="N171" t="n">
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -10215,7 +10215,7 @@
         <v>5</v>
       </c>
       <c r="N172" t="n">
-        <v>0.27</v>
+        <v>0.23</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -10271,7 +10271,7 @@
         <v>5</v>
       </c>
       <c r="N173" t="n">
-        <v>0.31</v>
+        <v>0.23</v>
       </c>
       <c r="O173" t="inlineStr"/>
       <c r="P173" t="inlineStr"/>
@@ -10323,7 +10323,7 @@
         <v>18</v>
       </c>
       <c r="N174" t="n">
-        <v>0.74</v>
+        <v>0.58</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -10379,7 +10379,7 @@
         <v>6</v>
       </c>
       <c r="N175" t="n">
-        <v>0.33</v>
+        <v>0.27</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -10439,7 +10439,7 @@
         <v>11</v>
       </c>
       <c r="N176" t="n">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -10499,7 +10499,7 @@
         <v>10</v>
       </c>
       <c r="N177" t="n">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -10559,7 +10559,7 @@
         <v>25</v>
       </c>
       <c r="N178" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.59</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -10615,7 +10615,7 @@
         <v>11</v>
       </c>
       <c r="N179" t="n">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -10671,7 +10671,7 @@
         <v>12</v>
       </c>
       <c r="N180" t="n">
-        <v>0.57</v>
+        <v>0.45</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -10727,7 +10727,7 @@
         <v>16</v>
       </c>
       <c r="N181" t="n">
-        <v>0.39</v>
+        <v>0.34</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -10783,7 +10783,7 @@
         <v>13</v>
       </c>
       <c r="N182" t="n">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
       <c r="O182" t="inlineStr">
         <is>
@@ -10839,7 +10839,7 @@
         <v>18</v>
       </c>
       <c r="N183" t="n">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -10951,7 +10951,7 @@
         <v>16</v>
       </c>
       <c r="N185" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
@@ -11007,7 +11007,7 @@
         <v>15</v>
       </c>
       <c r="N186" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -11063,7 +11063,7 @@
         <v>15</v>
       </c>
       <c r="N187" t="n">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -11231,7 +11231,7 @@
         <v>27</v>
       </c>
       <c r="N190" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -11343,7 +11343,7 @@
         <v>13</v>
       </c>
       <c r="N192" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -11399,7 +11399,7 @@
         <v>28</v>
       </c>
       <c r="N193" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="O193" t="inlineStr">
         <is>
@@ -11459,7 +11459,7 @@
         <v>17</v>
       </c>
       <c r="N194" t="n">
-        <v>0.39</v>
+        <v>0.41</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -11519,7 +11519,7 @@
         <v>15</v>
       </c>
       <c r="N195" t="n">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -11579,7 +11579,7 @@
         <v>15</v>
       </c>
       <c r="N196" t="n">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -11639,7 +11639,7 @@
         <v>14</v>
       </c>
       <c r="N197" t="n">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -11699,7 +11699,7 @@
         <v>14</v>
       </c>
       <c r="N198" t="n">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -11819,7 +11819,7 @@
         <v>24</v>
       </c>
       <c r="N200" t="n">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -11879,7 +11879,7 @@
         <v>12</v>
       </c>
       <c r="N201" t="n">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -11935,7 +11935,7 @@
         <v>12</v>
       </c>
       <c r="N202" t="n">
-        <v>0.44</v>
+        <v>0.37</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -11991,7 +11991,7 @@
         <v>11</v>
       </c>
       <c r="N203" t="n">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="O203" t="inlineStr"/>
       <c r="P203" t="inlineStr"/>
@@ -12043,7 +12043,7 @@
         <v>21</v>
       </c>
       <c r="N204" t="n">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -12099,7 +12099,7 @@
         <v>30</v>
       </c>
       <c r="N205" t="n">
-        <v>0.67</v>
+        <v>0.65</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -12155,7 +12155,7 @@
         <v>14</v>
       </c>
       <c r="N206" t="n">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -12211,7 +12211,7 @@
         <v>14</v>
       </c>
       <c r="N207" t="n">
-        <v>1.09</v>
+        <v>1.07</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -12267,7 +12267,7 @@
         <v>18</v>
       </c>
       <c r="N208" t="n">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -12323,7 +12323,7 @@
         <v>11</v>
       </c>
       <c r="N209" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -12379,7 +12379,7 @@
         <v>31</v>
       </c>
       <c r="N210" t="n">
-        <v>1.12</v>
+        <v>0.92</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -12435,7 +12435,7 @@
         <v>6</v>
       </c>
       <c r="N211" t="n">
-        <v>0.66</v>
+        <v>0.32</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -12491,7 +12491,7 @@
         <v>29</v>
       </c>
       <c r="N212" t="n">
-        <v>1</v>
+        <v>0.76</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -12547,7 +12547,7 @@
         <v>55</v>
       </c>
       <c r="N213" t="n">
-        <v>1.18</v>
+        <v>1.06</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -12603,7 +12603,7 @@
         <v>7</v>
       </c>
       <c r="N214" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -12659,7 +12659,7 @@
         <v>15</v>
       </c>
       <c r="N215" t="n">
-        <v>0.51</v>
+        <v>0.38</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -12715,7 +12715,7 @@
         <v>11</v>
       </c>
       <c r="N216" t="n">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -12771,7 +12771,7 @@
         <v>5</v>
       </c>
       <c r="N217" t="n">
-        <v>0.28</v>
+        <v>0.24</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -12827,7 +12827,7 @@
         <v>5</v>
       </c>
       <c r="N218" t="n">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="O218" t="inlineStr"/>
       <c r="P218" t="inlineStr"/>
@@ -12879,7 +12879,7 @@
         <v>5</v>
       </c>
       <c r="N219" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="O219" t="inlineStr"/>
       <c r="P219" t="inlineStr"/>
@@ -12931,7 +12931,7 @@
         <v>18</v>
       </c>
       <c r="N220" t="n">
-        <v>0.64</v>
+        <v>0.57</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -12987,7 +12987,7 @@
         <v>6</v>
       </c>
       <c r="N221" t="n">
-        <v>0.29</v>
+        <v>0.26</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -13047,7 +13047,7 @@
         <v>11</v>
       </c>
       <c r="N222" t="n">
-        <v>0.36</v>
+        <v>0.33</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -13107,7 +13107,7 @@
         <v>10</v>
       </c>
       <c r="N223" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -13167,7 +13167,7 @@
         <v>25</v>
       </c>
       <c r="N224" t="n">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -13279,7 +13279,7 @@
         <v>12</v>
       </c>
       <c r="N226" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -13391,7 +13391,7 @@
         <v>13</v>
       </c>
       <c r="N228" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -13559,7 +13559,7 @@
         <v>16</v>
       </c>
       <c r="N231" t="n">
-        <v>0.52</v>
+        <v>0.35</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -13615,7 +13615,7 @@
         <v>15</v>
       </c>
       <c r="N232" t="n">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -13671,7 +13671,7 @@
         <v>15</v>
       </c>
       <c r="N233" t="n">
-        <v>0.46</v>
+        <v>0.37</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -13727,7 +13727,7 @@
         <v>16</v>
       </c>
       <c r="N234" t="n">
-        <v>0.46</v>
+        <v>0.35</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -13783,7 +13783,7 @@
         <v>13</v>
       </c>
       <c r="N235" t="n">
-        <v>0.37</v>
+        <v>0.29</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -13839,7 +13839,7 @@
         <v>27</v>
       </c>
       <c r="N236" t="n">
-        <v>0.62</v>
+        <v>0.54</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -13895,7 +13895,7 @@
         <v>13</v>
       </c>
       <c r="N237" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -14007,7 +14007,7 @@
         <v>28</v>
       </c>
       <c r="N239" t="n">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -14247,7 +14247,7 @@
         <v>14</v>
       </c>
       <c r="N243" t="n">
-        <v>0.51</v>
+        <v>0.34</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -14427,7 +14427,7 @@
         <v>24</v>
       </c>
       <c r="N246" t="n">
-        <v>0.42</v>
+        <v>0.43</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -14543,7 +14543,7 @@
         <v>12</v>
       </c>
       <c r="N248" t="n">
-        <v>0.54</v>
+        <v>0.38</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -14599,7 +14599,7 @@
         <v>11</v>
       </c>
       <c r="N249" t="n">
-        <v>0.48</v>
+        <v>0.37</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -14655,7 +14655,7 @@
         <v>21</v>
       </c>
       <c r="N250" t="n">
-        <v>0.64</v>
+        <v>0.54</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -14711,7 +14711,7 @@
         <v>30</v>
       </c>
       <c r="N251" t="n">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -14767,7 +14767,7 @@
         <v>14</v>
       </c>
       <c r="N252" t="n">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -14823,7 +14823,7 @@
         <v>14</v>
       </c>
       <c r="N253" t="n">
-        <v>1.05</v>
+        <v>1.02</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -14879,7 +14879,7 @@
         <v>36</v>
       </c>
       <c r="N254" t="n">
-        <v>0.75</v>
+        <v>0.73</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -14935,7 +14935,7 @@
         <v>21</v>
       </c>
       <c r="N255" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -14991,7 +14991,7 @@
         <v>17</v>
       </c>
       <c r="N256" t="n">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -15103,7 +15103,7 @@
         <v>20</v>
       </c>
       <c r="N258" t="n">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -15215,7 +15215,7 @@
         <v>24</v>
       </c>
       <c r="N260" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -15271,7 +15271,7 @@
         <v>30</v>
       </c>
       <c r="N261" t="n">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -15327,7 +15327,7 @@
         <v>20</v>
       </c>
       <c r="N262" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -15439,7 +15439,7 @@
         <v>25</v>
       </c>
       <c r="N264" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -15495,7 +15495,7 @@
         <v>12</v>
       </c>
       <c r="N265" t="n">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -15551,7 +15551,7 @@
         <v>41</v>
       </c>
       <c r="N266" t="n">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -15611,7 +15611,7 @@
         <v>45</v>
       </c>
       <c r="N267" t="n">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -15667,7 +15667,7 @@
         <v>13</v>
       </c>
       <c r="N268" t="n">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -15779,7 +15779,7 @@
         <v>21</v>
       </c>
       <c r="N270" t="n">
-        <v>0.48</v>
+        <v>0.45</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -15835,7 +15835,7 @@
         <v>30</v>
       </c>
       <c r="N271" t="n">
-        <v>0.74</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -15891,7 +15891,7 @@
         <v>9</v>
       </c>
       <c r="N272" t="n">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -15947,7 +15947,7 @@
         <v>12</v>
       </c>
       <c r="N273" t="n">
-        <v>0.28</v>
+        <v>0.27</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -16059,7 +16059,7 @@
         <v>14</v>
       </c>
       <c r="N275" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
       <c r="O275" t="inlineStr">
         <is>
@@ -16171,7 +16171,7 @@
         <v>8</v>
       </c>
       <c r="N277" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="O277" t="inlineStr">
         <is>
@@ -16227,7 +16227,7 @@
         <v>13</v>
       </c>
       <c r="N278" t="n">
-        <v>0.29</v>
+        <v>0.31</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -16283,7 +16283,7 @@
         <v>15</v>
       </c>
       <c r="N279" t="n">
-        <v>0.34</v>
+        <v>0.31</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -16339,7 +16339,7 @@
         <v>15</v>
       </c>
       <c r="N280" t="n">
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -16395,7 +16395,7 @@
         <v>15</v>
       </c>
       <c r="N281" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -16451,7 +16451,7 @@
         <v>16</v>
       </c>
       <c r="N282" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -16507,7 +16507,7 @@
         <v>11</v>
       </c>
       <c r="N283" t="n">
-        <v>0.28</v>
+        <v>0.27</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -16563,7 +16563,7 @@
         <v>15</v>
       </c>
       <c r="N284" t="n">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -16619,7 +16619,7 @@
         <v>11</v>
       </c>
       <c r="N285" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -16675,7 +16675,7 @@
         <v>11</v>
       </c>
       <c r="N286" t="n">
-        <v>0.28</v>
+        <v>0.27</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -16731,7 +16731,7 @@
         <v>11</v>
       </c>
       <c r="N287" t="n">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -16787,7 +16787,7 @@
         <v>18</v>
       </c>
       <c r="N288" t="n">
-        <v>0.44</v>
+        <v>0.41</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -16843,7 +16843,7 @@
         <v>22</v>
       </c>
       <c r="N289" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -17011,7 +17011,7 @@
         <v>19</v>
       </c>
       <c r="N292" t="n">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="O292" t="inlineStr">
         <is>
@@ -17067,7 +17067,7 @@
         <v>24</v>
       </c>
       <c r="N293" t="n">
-        <v>1.1</v>
+        <v>1.08</v>
       </c>
       <c r="O293" t="inlineStr">
         <is>
@@ -17123,7 +17123,7 @@
         <v>13</v>
       </c>
       <c r="N294" t="n">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
       <c r="O294" t="inlineStr">
         <is>
@@ -17179,7 +17179,7 @@
         <v>21</v>
       </c>
       <c r="N295" t="n">
-        <v>1.06</v>
+        <v>1.02</v>
       </c>
       <c r="O295" t="inlineStr">
         <is>
@@ -17235,7 +17235,7 @@
         <v>18</v>
       </c>
       <c r="N296" t="n">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="O296" t="inlineStr">
         <is>
@@ -17291,7 +17291,7 @@
         <v>14</v>
       </c>
       <c r="N297" t="n">
-        <v>0.43</v>
+        <v>0.36</v>
       </c>
       <c r="O297" t="inlineStr">
         <is>
@@ -17347,7 +17347,7 @@
         <v>17</v>
       </c>
       <c r="N298" t="n">
-        <v>1.05</v>
+        <v>1.02</v>
       </c>
       <c r="O298" t="inlineStr">
         <is>
@@ -17403,7 +17403,7 @@
         <v>19</v>
       </c>
       <c r="N299" t="n">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="O299" t="inlineStr">
         <is>
@@ -17515,7 +17515,7 @@
         <v>20</v>
       </c>
       <c r="N301" t="n">
-        <v>1.03</v>
+        <v>1.01</v>
       </c>
       <c r="O301" t="inlineStr">
         <is>
@@ -17571,7 +17571,7 @@
         <v>18</v>
       </c>
       <c r="N302" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -17627,7 +17627,7 @@
         <v>14</v>
       </c>
       <c r="N303" t="n">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="O303" t="inlineStr">
         <is>
@@ -17683,7 +17683,7 @@
         <v>17</v>
       </c>
       <c r="N304" t="n">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="O304" t="inlineStr">
         <is>
@@ -17739,7 +17739,7 @@
         <v>19</v>
       </c>
       <c r="N305" t="n">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="O305" t="inlineStr">
         <is>
@@ -17851,7 +17851,7 @@
         <v>20</v>
       </c>
       <c r="N307" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="O307" t="inlineStr">
         <is>
@@ -17907,7 +17907,7 @@
         <v>18</v>
       </c>
       <c r="N308" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="O308" t="inlineStr">
         <is>
@@ -17963,7 +17963,7 @@
         <v>14</v>
       </c>
       <c r="N309" t="n">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
       <c r="O309" t="inlineStr">
         <is>
@@ -18019,7 +18019,7 @@
         <v>17</v>
       </c>
       <c r="N310" t="n">
-        <v>1.08</v>
+        <v>1</v>
       </c>
       <c r="O310" t="inlineStr">
         <is>
@@ -18075,7 +18075,7 @@
         <v>19</v>
       </c>
       <c r="N311" t="n">
-        <v>0.41</v>
+        <v>0.43</v>
       </c>
       <c r="O311" t="inlineStr">
         <is>
@@ -18131,7 +18131,7 @@
         <v>18</v>
       </c>
       <c r="N312" t="n">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="O312" t="inlineStr">
         <is>
@@ -18187,7 +18187,7 @@
         <v>20</v>
       </c>
       <c r="N313" t="n">
-        <v>1.2</v>
+        <v>0.98</v>
       </c>
       <c r="O313" t="inlineStr">
         <is>
@@ -18243,7 +18243,7 @@
         <v>17</v>
       </c>
       <c r="N314" t="n">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="O314" t="inlineStr">
         <is>
@@ -18355,7 +18355,7 @@
         <v>25</v>
       </c>
       <c r="N316" t="n">
-        <v>0.71</v>
+        <v>0.47</v>
       </c>
       <c r="O316" t="inlineStr">
         <is>
@@ -18411,7 +18411,7 @@
         <v>23</v>
       </c>
       <c r="N317" t="n">
-        <v>1.71</v>
+        <v>1.12</v>
       </c>
       <c r="O317" t="inlineStr">
         <is>
@@ -18467,7 +18467,7 @@
         <v>18</v>
       </c>
       <c r="N318" t="n">
-        <v>0.61</v>
+        <v>0.44</v>
       </c>
       <c r="O318" t="inlineStr">
         <is>
@@ -18523,7 +18523,7 @@
         <v>22</v>
       </c>
       <c r="N319" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.47</v>
       </c>
       <c r="O319" t="inlineStr">
         <is>
@@ -18579,7 +18579,7 @@
         <v>17</v>
       </c>
       <c r="N320" t="n">
-        <v>0.58</v>
+        <v>0.4</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -18635,7 +18635,7 @@
         <v>16</v>
       </c>
       <c r="N321" t="n">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="O321" t="inlineStr">
         <is>
@@ -18691,7 +18691,7 @@
         <v>25</v>
       </c>
       <c r="N322" t="n">
-        <v>0.47</v>
+        <v>0.45</v>
       </c>
       <c r="O322" t="inlineStr">
         <is>
@@ -18803,7 +18803,7 @@
         <v>17</v>
       </c>
       <c r="N324" t="n">
-        <v>0.46</v>
+        <v>0.41</v>
       </c>
       <c r="O324" t="inlineStr">
         <is>
@@ -18915,7 +18915,7 @@
         <v>20</v>
       </c>
       <c r="N326" t="n">
-        <v>1.08</v>
+        <v>1.03</v>
       </c>
       <c r="O326" t="inlineStr">
         <is>
@@ -19027,7 +19027,7 @@
         <v>21</v>
       </c>
       <c r="N328" t="n">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="O328" t="inlineStr">
         <is>
@@ -19083,7 +19083,7 @@
         <v>17</v>
       </c>
       <c r="N329" t="n">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="O329" t="inlineStr">
         <is>
@@ -19139,7 +19139,7 @@
         <v>21</v>
       </c>
       <c r="N330" t="n">
-        <v>0.6</v>
+        <v>0.44</v>
       </c>
       <c r="O330" t="inlineStr">
         <is>
@@ -19307,7 +19307,7 @@
         <v>28</v>
       </c>
       <c r="N333" t="n">
-        <v>1.5</v>
+        <v>1.16</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -19363,7 +19363,7 @@
         <v>22</v>
       </c>
       <c r="N334" t="n">
-        <v>0.95</v>
+        <v>0.43</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -19419,7 +19419,7 @@
         <v>29</v>
       </c>
       <c r="N335" t="n">
-        <v>0.78</v>
+        <v>0.51</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -19475,7 +19475,7 @@
         <v>21</v>
       </c>
       <c r="N336" t="n">
-        <v>0.66</v>
+        <v>0.46</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -19531,7 +19531,7 @@
         <v>26</v>
       </c>
       <c r="N337" t="n">
-        <v>1.25</v>
+        <v>1.08</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -19587,7 +19587,7 @@
         <v>23</v>
       </c>
       <c r="N338" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -19643,7 +19643,7 @@
         <v>28</v>
       </c>
       <c r="N339" t="n">
-        <v>1.34</v>
+        <v>1.11</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -19699,7 +19699,7 @@
         <v>22</v>
       </c>
       <c r="N340" t="n">
-        <v>0.55</v>
+        <v>0.44</v>
       </c>
       <c r="O340" t="inlineStr">
         <is>
@@ -19755,7 +19755,7 @@
         <v>29</v>
       </c>
       <c r="N341" t="n">
-        <v>0.55</v>
+        <v>0.51</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -19811,7 +19811,7 @@
         <v>17</v>
       </c>
       <c r="N342" t="n">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -19867,7 +19867,7 @@
         <v>21</v>
       </c>
       <c r="N343" t="n">
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -19979,7 +19979,7 @@
         <v>17</v>
       </c>
       <c r="N345" t="n">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="O345" t="inlineStr">
         <is>
@@ -20035,7 +20035,7 @@
         <v>20</v>
       </c>
       <c r="N346" t="n">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="O346" t="inlineStr">
         <is>
@@ -20091,7 +20091,7 @@
         <v>23</v>
       </c>
       <c r="N347" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -20147,7 +20147,7 @@
         <v>17</v>
       </c>
       <c r="N348" t="n">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -20203,7 +20203,7 @@
         <v>23</v>
       </c>
       <c r="N349" t="n">
-        <v>0.61</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -20259,7 +20259,7 @@
         <v>17</v>
       </c>
       <c r="N350" t="n">
-        <v>0.41</v>
+        <v>0.43</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -20315,7 +20315,7 @@
         <v>21</v>
       </c>
       <c r="N351" t="n">
-        <v>0.45</v>
+        <v>0.48</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -20371,7 +20371,7 @@
         <v>20</v>
       </c>
       <c r="N352" t="n">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -20483,7 +20483,7 @@
         <v>18</v>
       </c>
       <c r="N354" t="n">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -20539,7 +20539,7 @@
         <v>21</v>
       </c>
       <c r="N355" t="n">
-        <v>1.02</v>
+        <v>1.05</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -20595,7 +20595,7 @@
         <v>19</v>
       </c>
       <c r="N356" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -20651,7 +20651,7 @@
         <v>18</v>
       </c>
       <c r="N357" t="n">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -20763,7 +20763,7 @@
         <v>19</v>
       </c>
       <c r="N359" t="n">
-        <v>0.44</v>
+        <v>0.48</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -20875,7 +20875,7 @@
         <v>16</v>
       </c>
       <c r="N361" t="n">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -20987,7 +20987,7 @@
         <v>19</v>
       </c>
       <c r="N363" t="n">
-        <v>0.41</v>
+        <v>0.43</v>
       </c>
       <c r="O363" t="inlineStr">
         <is>
@@ -21099,7 +21099,7 @@
         <v>19</v>
       </c>
       <c r="N365" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -21155,7 +21155,7 @@
         <v>20</v>
       </c>
       <c r="N366" t="n">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -21211,7 +21211,7 @@
         <v>17</v>
       </c>
       <c r="N367" t="n">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="O367" t="inlineStr">
         <is>
@@ -21267,7 +21267,7 @@
         <v>18</v>
       </c>
       <c r="N368" t="n">
-        <v>0.51</v>
+        <v>0.45</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -21323,7 +21323,7 @@
         <v>18</v>
       </c>
       <c r="N369" t="n">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -21435,7 +21435,7 @@
         <v>17</v>
       </c>
       <c r="N371" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -21491,7 +21491,7 @@
         <v>20</v>
       </c>
       <c r="N372" t="n">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
       <c r="O372" t="inlineStr">
         <is>
@@ -21547,7 +21547,7 @@
         <v>16</v>
       </c>
       <c r="N373" t="n">
-        <v>1.07</v>
+        <v>1.02</v>
       </c>
       <c r="O373" t="inlineStr">
         <is>
@@ -21603,7 +21603,7 @@
         <v>20</v>
       </c>
       <c r="N374" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -21771,7 +21771,7 @@
         <v>18</v>
       </c>
       <c r="N377" t="n">
-        <v>0.54</v>
+        <v>0.4</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -21827,7 +21827,7 @@
         <v>20</v>
       </c>
       <c r="N378" t="n">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>
@@ -22051,7 +22051,7 @@
         <v>16</v>
       </c>
       <c r="N382" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="O382" t="inlineStr">
         <is>
@@ -22107,7 +22107,7 @@
         <v>19</v>
       </c>
       <c r="N383" t="n">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
       <c r="O383" t="inlineStr">
         <is>
@@ -22163,7 +22163,7 @@
         <v>18</v>
       </c>
       <c r="N384" t="n">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="O384" t="inlineStr">
         <is>
@@ -22275,7 +22275,7 @@
         <v>12</v>
       </c>
       <c r="N386" t="n">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
       <c r="O386" t="inlineStr">
         <is>
@@ -22331,7 +22331,7 @@
         <v>27</v>
       </c>
       <c r="N387" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.62</v>
       </c>
       <c r="O387" t="inlineStr">
         <is>
@@ -22387,7 +22387,7 @@
         <v>23</v>
       </c>
       <c r="N388" t="n">
-        <v>0.54</v>
+        <v>0.55</v>
       </c>
       <c r="O388" t="inlineStr">
         <is>
@@ -22503,7 +22503,7 @@
         <v>25</v>
       </c>
       <c r="N390" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="O390" t="inlineStr">
         <is>
@@ -22559,7 +22559,7 @@
         <v>18</v>
       </c>
       <c r="N391" t="n">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="O391" t="inlineStr"/>
       <c r="P391" t="inlineStr"/>
@@ -22580,17 +22580,17 @@
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>"Check out এইচ, টি, টি, পি, এস কোলন স্ল্যাশ, স্ল্যাশ subdomain ডট example ডট কম কোলন এইট জিরো এইট জিরো স্ল্যাশ path স্ল্যাশ to স্ল্যাশ page কোয়েশ্চেন মার্ক query একুয়াল ওয়ান"</t>
+          <t>"Check out এইচ, টি, টি, পি, এস কোলন স্ল্যাশ, স্ল্যাশ subdomain ডট example ডট কম কোলন এইট জিরো এইট জিরো স্ল্যাশ path স্ল্যাশ to স্ল্যাশ page কোয়েশ্চেন মার্ক query একুয়াল ওয়ান "</t>
         </is>
       </c>
       <c r="E392" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F392" t="n">
-        <v>0</v>
+        <v>0.0057</v>
       </c>
       <c r="G392" t="n">
-        <v>0</v>
+        <v>0.0645</v>
       </c>
       <c r="H392" t="n">
         <v>67</v>
@@ -22599,7 +22599,7 @@
         <v>174</v>
       </c>
       <c r="J392" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K392" t="n">
         <v>3</v>
@@ -22608,17 +22608,21 @@
         <v>31</v>
       </c>
       <c r="M392" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N392" t="n">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
       <c r="O392" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="P392" t="inlineStr"/>
+      <c r="P392" t="inlineStr">
+        <is>
+          <t>insert: '' → ' ' at 173-173</t>
+        </is>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
@@ -22723,7 +22727,7 @@
         <v>9</v>
       </c>
       <c r="N394" t="n">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="O394" t="inlineStr">
         <is>
@@ -22835,7 +22839,7 @@
         <v>6</v>
       </c>
       <c r="N396" t="n">
-        <v>0.36</v>
+        <v>0.39</v>
       </c>
       <c r="O396" t="inlineStr">
         <is>
@@ -22891,7 +22895,7 @@
         <v>6</v>
       </c>
       <c r="N397" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="O397" t="inlineStr">
         <is>
@@ -22947,7 +22951,7 @@
         <v>4</v>
       </c>
       <c r="N398" t="n">
-        <v>0.27</v>
+        <v>0.22</v>
       </c>
       <c r="O398" t="inlineStr">
         <is>
@@ -23003,7 +23007,7 @@
         <v>7</v>
       </c>
       <c r="N399" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="O399" t="inlineStr">
         <is>
@@ -23059,7 +23063,7 @@
         <v>7</v>
       </c>
       <c r="N400" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="O400" t="inlineStr">
         <is>
@@ -23162,11 +23166,11 @@
         <v>399</v>
       </c>
       <c r="B2" t="n">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>84.21%</t>
+          <t>83.96%</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -23182,10 +23186,10 @@
         <v>0.3029</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0112</v>
+        <v>0.0114</v>
       </c>
       <c r="I2" t="n">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
       <c r="J2" t="n">
         <v>384</v>
@@ -23272,7 +23276,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="3">
@@ -23294,7 +23298,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.88</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="4">
@@ -23316,7 +23320,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5">
@@ -23338,7 +23342,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3490909090909091</v>
+        <v>0.2959090909090909</v>
       </c>
     </row>
     <row r="6">
@@ -23360,7 +23364,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.325</v>
+        <v>0.315</v>
       </c>
     </row>
     <row r="7">
@@ -23382,7 +23386,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.67</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="8">
@@ -23404,7 +23408,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="9">
@@ -23448,7 +23452,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="11">
@@ -23470,7 +23474,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.58</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="12">
@@ -23492,7 +23496,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7324999999999999</v>
+        <v>0.6675</v>
       </c>
     </row>
     <row r="13">
@@ -23514,7 +23518,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="14">
@@ -23536,7 +23540,7 @@
         <v>0.05283</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3996666666666667</v>
+        <v>0.365</v>
       </c>
     </row>
     <row r="15">
@@ -23558,7 +23562,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5939024390243902</v>
+        <v>0.5557723577235772</v>
       </c>
     </row>
     <row r="16">
@@ -23580,7 +23584,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8099999999999999</v>
+        <v>0.696</v>
       </c>
     </row>
     <row r="17">
@@ -23602,7 +23606,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7600000000000001</v>
+        <v>0.7733333333333333</v>
       </c>
     </row>
     <row r="18">
@@ -23646,7 +23650,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.282</v>
+        <v>0.264</v>
       </c>
     </row>
     <row r="20">
@@ -23668,7 +23672,7 @@
         <v>0.12208125</v>
       </c>
       <c r="F20" t="n">
-        <v>0.755625</v>
+        <v>0.7175</v>
       </c>
     </row>
     <row r="21">
@@ -23690,7 +23694,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="22">
@@ -23712,7 +23716,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.492</v>
+        <v>0.4773333333333333</v>
       </c>
     </row>
     <row r="23">
@@ -23734,7 +23738,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="24">
@@ -23756,7 +23760,7 @@
         <v>0.04207058823529412</v>
       </c>
       <c r="F24" t="n">
-        <v>0.2705882352941176</v>
+        <v>0.2535294117647059</v>
       </c>
     </row>
     <row r="25">
@@ -23800,7 +23804,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.64</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="27">
@@ -23822,7 +23826,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.3566666666666666</v>
+        <v>0.3633333333333333</v>
       </c>
     </row>
     <row r="28">
@@ -23844,7 +23848,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.7300000000000001</v>
+        <v>0.7225</v>
       </c>
     </row>
     <row r="29">
@@ -23866,7 +23870,7 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.275</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="30">
@@ -23879,16 +23883,16 @@
         <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>0.001425</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>0.016125</v>
       </c>
       <c r="F30" t="n">
-        <v>0.6325</v>
+        <v>0.6225000000000001</v>
       </c>
     </row>
     <row r="31">
@@ -23910,7 +23914,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.31</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="32">
@@ -23932,7 +23936,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.2483333333333333</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="33">
@@ -23954,7 +23958,7 @@
         <v>0.001448913043478261</v>
       </c>
       <c r="F33" t="n">
-        <v>0.696195652173913</v>
+        <v>0.5970652173913044</v>
       </c>
     </row>
     <row r="34">
@@ -23976,7 +23980,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="35">
@@ -23998,7 +24002,7 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.41</v>
+        <v>0.405</v>
       </c>
     </row>
     <row r="36">
@@ -24042,7 +24046,7 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0.2585714285714286</v>
+        <v>0.2528571428571428</v>
       </c>
     </row>
   </sheetData>
@@ -24056,7 +24060,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25868,6 +25872,34 @@
         </is>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>391</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>"Check out https://subdomain.example.com:8080/path/to/page?query=1"</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>"Check out এইচ, টি, টি, পি, এস কোলন স্ল্যাশ, স্ল্যাশ subdomain ডট example ডট কম কোলন এইট জিরো এইট জিরো স্ল্যাশ path স্ল্যাশ to স্ল্যাশ page কোয়েশ্চেন মার্ক query একুয়াল ওয়ান"</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>"Check out এইচ, টি, টি, পি, এস কোলন স্ল্যাশ, স্ল্যাশ subdomain ডট example ডট কম কোলন এইট জিরো এইট জিরো স্ল্যাশ path স্ল্যাশ to স্ল্যাশ page কোয়েশ্চেন মার্ক query একুয়াল ওয়ান "</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>0.0057</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>insert: '' → ' ' at 173-173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>